<commit_message>
Fixed typos, added new test cases.
Signed-off-by: raviv <ravivkomem@gmail.com>
</commit_message>
<xml_diff>
--- a/‏‏G1_Acceptance.Ass1.xlsx
+++ b/‏‏G1_Acceptance.Ass1.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leehu\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raviv Komem\Desktop\Project Copy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F9AC811-D531-4313-A5EE-38363B2DDEC8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9A1B13E-F06C-4B1A-A91F-C8C96609D775}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{CBCEEB33-43CF-45A0-956C-B39C2D4E436E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CBCEEB33-43CF-45A0-956C-B39C2D4E436E}"/>
   </bookViews>
   <sheets>
     <sheet name="request submission" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="56">
   <si>
     <t>Comments</t>
   </si>
@@ -58,9 +58,6 @@
   </si>
   <si>
     <t>איתי דוד - itaydavid22@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">רביב קומם - </t>
   </si>
   <si>
     <t xml:space="preserve">ליאור קאופמן - </t>
@@ -80,6 +77,27 @@
   </si>
   <si>
     <t>RequestSubmissionSucssesful</t>
+  </si>
+  <si>
+    <t>RequestSubmissionWithDocumentsSucssesful</t>
+  </si>
+  <si>
+    <t>The System selected dosen't exist</t>
+  </si>
+  <si>
+    <t>No existing situation typed</t>
+  </si>
+  <si>
+    <t>No change discription typed</t>
+  </si>
+  <si>
+    <t>No reason typed</t>
+  </si>
+  <si>
+    <t>The request is empty</t>
+  </si>
+  <si>
+    <t>רביב קומם - ravivkomem@gmail;.com</t>
   </si>
   <si>
     <t>open the change request page:
@@ -88,11 +106,7 @@
 "My courses aren't sorted by alphbetical order"
 3.In change description field, type "I would like an option to see my courses sorted by alphabetical order"
 4. In reason field type "It would help me to find a specific course faster"
-5. Click "Uplode" button</t>
-  </si>
-  <si>
-    <t>A new request has been received by the system and a request ID was presented 
-to the customer.</t>
+5. Click "Submit" button</t>
   </si>
   <si>
     <t>open the change request page:
@@ -102,48 +116,61 @@
 3.In change description field, type "I would like an option to see my courses sorted by alphabetical order"
 4. In reason field type "It would help me to find a specific course faster"
 5. Click "upload documents" button
-6. Add a screenshot of the existing situation
-7. Click "Upload" button</t>
+6. Add a screenshot of the existing situation (JPEG format)
+7. Click "Submit" button</t>
+  </si>
+  <si>
+    <t>A new request has been received by the system and a request ID was presented 
+to the user.</t>
   </si>
   <si>
     <t>A new request has been received by the system and
 the screenshot was successfully uploaded and
-a request ID was presented to the customer.</t>
-  </si>
-  <si>
-    <t>The user exists on the system. 
-The subsystem that the user chose exists.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The user exists on the system. 
+a request ID was presented to the user.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User is logged in to the system.
 The subsystem that the user chose exists.
 </t>
   </si>
   <si>
-    <t>The user exists on the system. 
+    <t>User is logged in to the system. 
 The subsystem that the user chose exists.
 The screenshot is on the user computer.</t>
   </si>
   <si>
-    <t>RequestSubmissionWithDocumentsSucssesful</t>
-  </si>
-  <si>
-    <t>RequestSubmissionWrongDetailsFaild</t>
+    <t>User is logged in to the system. 
+The subsystem that the user chose exists.</t>
+  </si>
+  <si>
+    <t>User is logged in to the system.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The system throws out 
+a warning message "Must fill all the required fields"
+the missing field is marked in red
+</t>
+  </si>
+  <si>
+    <t>The system throws out 
+a warning message "Invalid system name"
+the problematic field is marked in red</t>
   </si>
   <si>
     <r>
       <t xml:space="preserve">open the change request page:
-1. </t>
-    </r>
-    <r>
-      <rPr>
+1. choose a system: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Don't choose a system</t>
+      <t>Greg</t>
     </r>
     <r>
       <rPr>
@@ -159,23 +186,69 @@
 "My courses aren't sorted by alphbetical order"
 3.In change description field, type "I would like an option to see my courses sorted by alphabetical order"
 4. In reason field type "It would help me to find a specific course faster"
-5. Click "Uplode" button</t>
-    </r>
+5. Click "Submit" button</t>
+    </r>
+  </si>
+  <si>
+    <t>User is logged in to the system.
+Greg is not a valid system.</t>
+  </si>
+  <si>
+    <t>RequestSubmissionSubsystemFailed</t>
+  </si>
+  <si>
+    <t>RequestSubmissionInvalidSubsystemFail</t>
+  </si>
+  <si>
+    <t>RequestSubmissionExitingSituationFailed</t>
   </si>
   <si>
     <r>
       <t xml:space="preserve">open the change request page:
-1. choose a system: </t>
-    </r>
-    <r>
-      <rPr>
+1. Choose a system: moodle
+2. In existing situation field: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Greg</t>
+      <t>Don't type anything</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="177"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+3.In change description field, type "I would like an option to see my courses sorted by alphabetical order"
+4. In reason field type "It would help me to find a specific course faster"
+5. Click "Submit" button</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">open the change request page:
+1. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Don't choose a system</t>
     </r>
     <r>
       <rPr>
@@ -191,83 +264,13 @@
 "My courses aren't sorted by alphbetical order"
 3.In change description field, type "I would like an option to see my courses sorted by alphabetical order"
 4. In reason field type "It would help me to find a specific course faster"
-5. Click "Uplode" button</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">The system throws out 
-a warning message "No
- system was selected so
- the request cannot be 
-uploaded"
-the missing field is marked in red
-</t>
+5. Click "Submit" button</t>
+    </r>
   </si>
   <si>
     <t>The system throws out 
-a warning message "The selected system does not exist so the request cannot be uploaded"
-the problematic field is marked in red</t>
-  </si>
-  <si>
-    <t>The System selected dosen't exist</t>
-  </si>
-  <si>
-    <t>RequestSubmissionSubsystemFaild</t>
-  </si>
-  <si>
-    <t>RequestSubmissionExitingSituationFaild</t>
-  </si>
-  <si>
-    <r>
-      <t>open the change request page:
-1. Choose a system: moodle
-2. In existing situation field:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Don't type anything</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="177"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-3.In change description field, type "I would like an option to see my courses sorted by alphabetical order"
-4. In reason field type "It would help me to find a specific course faster"
-5. Click "Uplode" button</t>
-    </r>
-  </si>
-  <si>
-    <t>The system throws out 
-a warning message "No
- exisiting situation was typed so the request cannot be uploaded"
+a warning message "Must fill all the required fields"
 the missing field is marked in red</t>
-  </si>
-  <si>
-    <t>No existing situation typed</t>
-  </si>
-  <si>
-    <t>RequestSubmissionChangeDescriptionFaild</t>
-  </si>
-  <si>
-    <t>The system throws out 
-a warning message "No
-change description was typed so the request cannot be uploaded"
-the missing field is marked in red</t>
-  </si>
-  <si>
-    <t>No change discription typed</t>
   </si>
   <si>
     <r>
@@ -279,6 +282,7 @@
     </r>
     <r>
       <rPr>
+        <b/>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
         <rFont val="Arial"/>
@@ -298,11 +302,11 @@
       </rPr>
       <t xml:space="preserve">
 4. In reason field type "It would help me to find a specific course faster"
-5. Click "Uplode" button</t>
-    </r>
-  </si>
-  <si>
-    <t>RequestSubmissionReasonFaild</t>
+5. Click "Submit" button</t>
+    </r>
+  </si>
+  <si>
+    <t>RequestSubmissionChangeDescriptionFailed</t>
   </si>
   <si>
     <r>
@@ -315,6 +319,7 @@
     </r>
     <r>
       <rPr>
+        <b/>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
         <rFont val="Arial"/>
@@ -333,38 +338,177 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-5. Click "Uplode" button</t>
+5. Click "Submit" button</t>
+    </r>
+  </si>
+  <si>
+    <t>RequestSubmissionEmptyFailed</t>
+  </si>
+  <si>
+    <r>
+      <t>Open the change request page:
+1.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Leave all the fields empty</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="177"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2. Click "Submit" button</t>
     </r>
   </si>
   <si>
     <t>The system throws out 
-a warning message "No
-reason was typed so the request cannot be uploaded"
-the missing field is marked in red</t>
-  </si>
-  <si>
-    <t>No reason typed</t>
-  </si>
-  <si>
-    <t>RequestSubmissionEmptyFaild</t>
-  </si>
-  <si>
-    <t>open the change request page:
-1. Click "Uplode" button</t>
+a warning message "Must fill all the required fields"
+All required fields are marked in red</t>
+  </si>
+  <si>
+    <t>DocumentTypeNotSupportedFail</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">open the change request page:
+1. Choose a system: moodle
+2. In existing situation field, type
+"My courses aren't sorted by alphbetical order"
+3.In change description field, type "I would like an option to see my courses sorted by alphabetical order"
+4. In reason field type "It would help me to find a specific course faster"
+5. Click "upload documents" button
+6. Add an </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>EXE File</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="177"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+7. Click "Submit" button</t>
+    </r>
+  </si>
+  <si>
+    <t>DocumentExceedVolumeFail</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">open the change request page:
+1. Choose a system: moodle
+2. In existing situation field, type
+"My courses aren't sorted by alphbetical order"
+3.In change description field, type "I would like an option to see my courses sorted by alphabetical order"
+4. In reason field type "It would help me to find a specific course faster"
+5. Click "upload documents" button
+6. Add Alegbra Course Syllabus PDF </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(21MB)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="177"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+7. Click "Submit" button</t>
+    </r>
   </si>
   <si>
     <t>The system throws out 
-a warning message "No
- system was selected so
- the request cannot be 
-uploaded"
-All the missing fields are marked in red</t>
-  </si>
-  <si>
-    <t>The request is empty</t>
-  </si>
-  <si>
-    <t>The user exists on the system.</t>
+a warning message "File too large"
+Uploaded file is deleted from the form.</t>
+  </si>
+  <si>
+    <t>The system throws out 
+a warning message "Only JPEG / PDF files are allowed"
+Uploaded file is deleted from the form.</t>
+  </si>
+  <si>
+    <t>DocumentQuantityOverLimitFail</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">open the change request page:
+1. Choose a system: moodle
+2. In existing situation field, type
+"My courses aren't sorted by alphbetical order"
+3.In change description field, type "I would like an option to see my courses sorted by alphabetical order"
+4. In reason field type "It would help me to find a specific course faster"
+5. Click "upload documents" button
+6. Upload </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="177"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> JPEG Files
+7. Click "Submit" button</t>
+    </r>
+  </si>
+  <si>
+    <t>The system throws out 
+a warning message "Only 3 files are allowed"
+The last uploaded file is deleted from the form.</t>
+  </si>
+  <si>
+    <t>RequestSubmissionChangeReasonFailed</t>
   </si>
 </sst>
 </file>
@@ -381,6 +525,7 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
@@ -408,11 +553,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -421,9 +563,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -739,227 +878,228 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6588D779-DA2D-4DE3-9387-6E8C06BB5375}">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A18" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A15" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.4140625" customWidth="1"/>
-    <col min="2" max="2" width="28.25" customWidth="1"/>
-    <col min="3" max="3" width="23.08203125" customWidth="1"/>
-    <col min="4" max="4" width="27" customWidth="1"/>
-    <col min="5" max="5" width="39.25" customWidth="1"/>
+    <col min="1" max="1" width="31.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.25" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="42.375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="40.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F10" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="184" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>16</v>
+    <row r="11" spans="1:6" ht="183.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F11" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="239.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>18</v>
+    <row r="12" spans="1:6" ht="185.25" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="F12" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="184" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>25</v>
+    <row r="13" spans="1:6" ht="183.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="F13" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="188.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>26</v>
+    <row r="14" spans="1:6" ht="188.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="F14" s="2">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="193" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>32</v>
+    <row r="15" spans="1:6" ht="192.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="F15" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="188.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>38</v>
+    <row r="16" spans="1:6" ht="188.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>40</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="F16" s="2">
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="168.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
+    <row r="17" spans="1:6" ht="168.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>40</v>
-      </c>
       <c r="E17" s="2" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="F17" s="2">
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="118" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C18" s="4" t="s">
+    <row r="18" spans="1:6" ht="117.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="3" t="s">
         <v>44</v>
       </c>
       <c r="E18" s="2" t="s">
@@ -969,9 +1109,58 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
+    <row r="19" spans="1:6" ht="171.75" x14ac:dyDescent="0.2">
+      <c r="A19" s="2"/>
+      <c r="B19" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F19" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="171.75" x14ac:dyDescent="0.2">
+      <c r="A20" s="2"/>
+      <c r="B20" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F20" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="171.75" x14ac:dyDescent="0.2">
+      <c r="B21" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F21" s="1">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>